<commit_message>
Update Shot Classification Models.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Shot Classification Results/Shot Classification Models.xlsx
+++ b/Documentation/Shot Classification Results/Shot Classification Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umair\Documents\GitHub\ShotSense\Documentation\Shot Classification Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DD2A68-2B27-4BD2-A13B-54F0122EFBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE52180-78DA-4B43-9581-D410F57EB213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B867722E-1A22-4D5D-A785-8333682FAF9F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Model Architecture</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Pre-Trained Model</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -212,9 +215,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -224,12 +225,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -239,9 +236,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -257,9 +252,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -269,15 +263,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D289C28B-A594-4DE4-A82A-7EA0A76799D9}">
-  <dimension ref="C4:O24"/>
+  <dimension ref="B4:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,269 +607,239 @@
     <col min="15" max="15" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="11" t="s">
+    <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="3:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="4" t="s">
+    </row>
+    <row r="6" spans="2:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="16">
+        <v>45246</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <v>0.61280000000000001</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>0.52500000000000002</v>
       </c>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="3:15" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="4"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="1"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C8" s="4"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="1"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C9" s="4"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="1"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="1"/>
+    </row>
+    <row r="7" spans="2:15" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="4"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="4"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="4"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="4"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="4"/>
       <c r="O9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C10" s="4"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="1"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C11" s="4"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="1"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C12" s="4"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="1"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C13" s="4"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="1"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C14" s="4"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="1"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C15" s="4"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="1"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C16" s="4"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="1"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C17" s="4"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="1"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C18" s="4"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="1"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C19" s="4"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="1"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C20" s="4"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="1"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="4"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="4"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="4"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="4"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="4"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="4"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="4"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="4"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="4"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="4"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="4"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="4"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="4"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="4"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="4"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="4"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="4"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="3"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="4"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="4"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="5"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="1"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="E24" s="14" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="7"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="7"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="E24" s="10" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>